<commit_message>
save local edits before rebase
</commit_message>
<xml_diff>
--- a/CRM Analyst.xlsx
+++ b/CRM Analyst.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7110" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7110" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="VIP BUYER" sheetId="2" r:id="rId1"/>
@@ -1374,7 +1374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
@@ -2334,7 +2334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -3395,7 +3395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -3454,8 +3454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DH22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>